<commit_message>
ECOSCOM-4453 - Create group action to export records to excel Changes according to the pull request comments
</commit_message>
<xml_diff>
--- a/ecos-base-core-repo/src/main/resources/alfresco/templates/reports/ru/citeck/default.xlsx
+++ b/ecos-base-core-repo/src/main/resources/alfresco/templates/reports/ru/citeck/default.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Eclipse-EcoS\idocs-core\idocs-repo\config\alfresco\extension\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRep\ecos-community-core\ecos-base-core-repo\src\main\resources\alfresco\templates\reports\ru\citeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="367" yWindow="14" windowWidth="17171" windowHeight="6398"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="17175" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>title</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +415,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="9" customWidth="1"/>
   </cols>
@@ -429,9 +426,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
ECOSCOM-4470 - Change records Iterable strategy for group actions
</commit_message>
<xml_diff>
--- a/ecos-base-core-repo/src/main/resources/alfresco/templates/reports/ru/citeck/default.xlsx
+++ b/ecos-base-core-repo/src/main/resources/alfresco/templates/reports/ru/citeck/default.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Eclipse-EcoS\idocs-core\idocs-repo\config\alfresco\extension\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRep\ecos-community-core\ecos-base-core-repo\src\main\resources\alfresco\templates\reports\ru\citeck\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="367" yWindow="14" windowWidth="17171" windowHeight="6398"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="17175" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>title</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +415,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="9" customWidth="1"/>
   </cols>
@@ -429,9 +426,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>